<commit_message>
updated new features and experiments tha didnt take off
</commit_message>
<xml_diff>
--- a/datasets/loanCompetition/FE_scores.xlsx
+++ b/datasets/loanCompetition/FE_scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malfaro\Desktop\mae_code\projects_2020\Framework\datasets\loanCompetition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A578765-EF3C-471C-B7E7-A1192534C47F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C54A53-7148-4898-8C12-FD9668BEB361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48F773C9-F6FA-4D5D-946A-F989BEDBE3E8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -57,13 +57,40 @@
   </si>
   <si>
     <t>FE_5</t>
+  </si>
+  <si>
+    <t>FE_0</t>
+  </si>
+  <si>
+    <t>FE_6</t>
+  </si>
+  <si>
+    <t>FE_7</t>
+  </si>
+  <si>
+    <t>FE_8</t>
+  </si>
+  <si>
+    <t>FE_9</t>
+  </si>
+  <si>
+    <t>FE_10</t>
+  </si>
+  <si>
+    <t>ROC_AUC</t>
+  </si>
+  <si>
+    <t>RandomForest</t>
+  </si>
+  <si>
+    <t>Correl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +103,18 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,10 +152,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,81 +477,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ADB519-331E-45CE-BC07-7801D6565A99}">
-  <dimension ref="A5:F7"/>
+  <dimension ref="A5:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
         <v>0.72495799999999999</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>0.73109999999999997</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.74938000000000005</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>0.75151000000000001</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.76178999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
         <v>0.82289000000000001</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.82489999999999997</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.82289000000000001</v>
       </c>
       <c r="E7" s="1">
         <v>0.82289000000000001</v>
       </c>
       <c r="F7" s="1">
+        <v>0.82289000000000001</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.81677</v>
       </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.80479999999999996</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.78410000000000002</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.79496999999999995</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.79535800000000001</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.80218</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.80279999999999996</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>